<commit_message>
Stability Updates for ANN and Minor Rework for demo
</commit_message>
<xml_diff>
--- a/Chatbot/Queries/General Queries.xlsx
+++ b/Chatbot/Queries/General Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Study\Current\Minor Project\minor_project\Chatbot_Final\Queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4E72FF-FC24-4E58-9090-D623AF755276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B617989C-829E-4E5C-8D8B-CF4A7C284A58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A03034D1-1D50-4DFB-AB94-E23ACBEFD145}"/>
   </bookViews>
@@ -54,22 +54,22 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>Who is the President of this College?, Who is the head of this University?, What is the name of the President of Manipal University Jaipur?, Who is the Dead of this College?, Does this college have a head?</t>
-  </si>
-  <si>
     <t>The more details about board of management can be found at https://jaipur.manipal.edu/muj/about-us/board-of-management.html</t>
   </si>
   <si>
     <t>Timings</t>
   </si>
   <si>
-    <t>What is the timing of the College?, What time the college is open?, May I know the time I can contact Manipal University Jaipur?, How long the college will stay open?</t>
-  </si>
-  <si>
     <t>The College timings are 9:00 to 18:00 in Indian Standard Time (IST)</t>
   </si>
   <si>
-    <t>Manipal University Jaipur, Dehmi Kalan, Off Jaipur-Ajmer Expressway, Jaipur, (Raj.) Rajasthan 303007. Phone: +91 141-3999100 More details can be found on: https://jaipur.manipal.edu/muj/contact-us.html</t>
+    <t>The University is located at, Manipal University Jaipur, Dehmi Kalan, Off Jaipur-Ajmer Expressway, Jaipur, (Raj.) Rajasthan 303007. Phone: +91 141-3999100 More details can be found on: https://jaipur.manipal.edu/muj/contact-us.html</t>
+  </si>
+  <si>
+    <t>What is the timing of the College?, What time the college is open?, May I know the time I can contact Manipal University Jaipur?, How long the college will stay open?, What are the timings of MUJ?, At what time is the college open?, What is the time I can contact the University?</t>
+  </si>
+  <si>
+    <t>Who is the President of this College?, Who is the head of this University?, What is the name of the President of Manipal University Jaipur?, Who is the Dead of this College?, Does this college have a head?, Who is the head of this College?, Who are the managers of Manipal University Jaipur?, Who is the President of MUJ?, Who is the president of this University?, Is there a board of directors in this college?</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -467,29 +467,29 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More General Queries Added
Might have to modify the network for even further queries.
</commit_message>
<xml_diff>
--- a/Chatbot/Queries/General Queries.xlsx
+++ b/Chatbot/Queries/General Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Study\Current\Minor Project\minor_project\Chatbot_Final\Queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B617989C-829E-4E5C-8D8B-CF4A7C284A58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C53AC0-3ABC-410F-8000-C52142A8BCBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A03034D1-1D50-4DFB-AB94-E23ACBEFD145}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Query</t>
   </si>
@@ -54,22 +54,118 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>The more details about board of management can be found at https://jaipur.manipal.edu/muj/about-us/board-of-management.html</t>
-  </si>
-  <si>
     <t>Timings</t>
   </si>
   <si>
     <t>The College timings are 9:00 to 18:00 in Indian Standard Time (IST)</t>
   </si>
   <si>
-    <t>The University is located at, Manipal University Jaipur, Dehmi Kalan, Off Jaipur-Ajmer Expressway, Jaipur, (Raj.) Rajasthan 303007. Phone: +91 141-3999100 More details can be found on: https://jaipur.manipal.edu/muj/contact-us.html</t>
-  </si>
-  <si>
     <t>What is the timing of the College?, What time the college is open?, May I know the time I can contact Manipal University Jaipur?, How long the college will stay open?, What are the timings of MUJ?, At what time is the college open?, What is the time I can contact the University?</t>
   </si>
   <si>
     <t>Who is the President of this College?, Who is the head of this University?, What is the name of the President of Manipal University Jaipur?, Who is the Dead of this College?, Does this college have a head?, Who is the head of this College?, Who are the managers of Manipal University Jaipur?, Who is the President of MUJ?, Who is the president of this University?, Is there a board of directors in this college?</t>
+  </si>
+  <si>
+    <t>Affiliations</t>
+  </si>
+  <si>
+    <t>The University is located at, 
+Manipal University Jaipur, 
+Dehmi Kalan, 
+Off Jaipur-Ajmer Expressway, 
+Jaipur, (Raj.) Rajasthan 303007. Phone: +91 141-3999100 
+More details can be found at: https://jaipur.manipal.edu/muj/contact-us.html</t>
+  </si>
+  <si>
+    <t>The more details about Board of Management can be found at: 
+https://jaipur.manipal.edu/muj/about-us/board-of-management.html</t>
+  </si>
+  <si>
+    <t>Manipal University Jaipur is Affiliated with UGC, NAAC (with A+ score) and AICTE. More information can be found at: https://jaipur.manipal.edu/muj/about-us/recognitions-and-accreditations.html</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>What are the courses offered in this college?, What courses does MUJ offer?, What  courses can I do here?, What Graudation can I do from here?, Does this college have ?, What courses are offered in MUJ?, Do you know about the courses in MUJ?, Do you have a list of Courses available are MUJ?, How many courses does Manipal University Jaipur offer?</t>
+  </si>
+  <si>
+    <t>Manipal University Jaipur offers many courses like B.Tech., M.Tech., Law, Arts, Fashion Design, Management and much more. To know more about the Courses please go to: https://jaipur.manipal.edu/muj/academics.html</t>
+  </si>
+  <si>
+    <t>Faculties</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>More Information at: https://jaipur.manipal.edu/muj/research.html</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>Calender</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Fee information can be found at: https://jaipur.manipal.edu/muj/admission/indian-students/fees.html</t>
+  </si>
+  <si>
+    <t>Clubs</t>
+  </si>
+  <si>
+    <t>Information on Clubs can be found at: https://jaipur.manipal.edu/muj/life-at-muj/Student-CLUBS.html</t>
+  </si>
+  <si>
+    <t>Placements</t>
+  </si>
+  <si>
+    <t>What are the acreditations of MUJ?, What are the Recognitions of Manipal University Jaipur?, What awards does this University hold?, Is the University UGC Affiliated?, What affiliations does this College have?, What are the awards given to this college?, Tell me the accreditations of this College.</t>
+  </si>
+  <si>
+    <t>What are the Faculties of this College?, What departments does this college have?, What are the different Schools in this college?, Tell me about the departments of the college, Name the departments of Manipal University Jaipur, How many departments does MUJ have?</t>
+  </si>
+  <si>
+    <t>The different courses are grouped into different Faculties each of which contain their respective Schools, and the Schools are groups of similar departments. More information at: https://jaipur.manipal.edu/muj/academics/institution-list.html</t>
+  </si>
+  <si>
+    <t>More Information about MUJ Administration at: https://jaipur.manipal.edu/muj/about-us/administration.html</t>
+  </si>
+  <si>
+    <t>How can I contact finance department?, I need to know more about the administration of this college., Can I know more about the Administration department?, What can you tell me about the Administration Department?, How many administration departments are there?, Can I know more about the Finance Department?, What can you tell me about the Human Resource Department?, How is the HR management of the college.</t>
+  </si>
+  <si>
+    <t>What are the research options available at MUJ?, What are the facilities available at Manipal University?, Can I do research from this University?, I want to know more about Research in MUJ, May I know more about Research in MUJ?, Do you know about Research facilities available in MUJ?, I would like to know more about PhD in this college, Can I apply for my Doctorate in MUJ?, I would like to know more about Doctor of Philosophy options available in Manipal.</t>
+  </si>
+  <si>
+    <t>What are the facilities available to Students in Manipal?, What are the facilities available for parents looking to stay at MUJ?, Can I know more about Hostel and Mess in MUJ?, What are the shops and food facilities available in MUJ?, Can I buy books in MUJ?, Does this College have a Library?, Do we have a Gym or any Sports Facilities available in MUJ?,What are the sports and extracurricular facilities available in MUJ?</t>
+  </si>
+  <si>
+    <t>Can I know the important dates of this semester?, Where can I find the Academic Calender of this year?, What are the holidays of this semester?, Do you have a link to Academic Calender?, What can you tell me about the academic schedule of this year?, I would like to know about the holidays this year, What are the exam dates of this semester?, Can I know the last date of registration of this semester?, When are the mid term exams of this semester?</t>
+  </si>
+  <si>
+    <t>Calender of Holidays and Academic events can be found at: https://jaipur.manipal.edu/muj/academics/Academic-Calender.html</t>
+  </si>
+  <si>
+    <t>Manipal University Jaipur provides lots of facilities in various fields, for information check out: https://jaipur.manipal.edu/muj/life-at-muj/campus-facilities.html</t>
+  </si>
+  <si>
+    <t>What are the fees for students?, What are the entrance fees for first year students in MUJ?, Can I know my fees for second year?, I need to know details about fees of my branch., I want to know the amount I have to pay for my college tuition in Manipal University Jaipur, I want to pay my fees but I don't know the amount, can I know the fees for first year?</t>
+  </si>
+  <si>
+    <t>What clubs do students have in Manipal?, What are the local organizations formed by students in MUJ?, What do you know about extracurricular activities held by clubs?, Do you know about different clubs in MUJ?, I would like to know about student clubs in Manipal.</t>
+  </si>
+  <si>
+    <t>Do you have placement statistics from last year?, I would like to know about last year placements, What placements have the students got last year?, What do you know about placements in Engineering?, Can I know more about placement Opportunities at MUJ?, Can I know more about hiring in MUJ?, Can I have the details about Jobs and Placements?, I would like to know about hiring status of MUJ, What companies come for hiring in MUJ?</t>
+  </si>
+  <si>
+    <t>Various Technical Companies like Dell, Microsoft, Adobe and HP come for hiring at MUJ Campus. Detailed Information about Placements can be found at: https://jaipur.manipal.edu/muj/admission/placement-training.html</t>
   </si>
 </sst>
 </file>
@@ -113,13 +209,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50D50E5-4F3F-42FD-8CE3-091B0116DDAB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,37 +564,147 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>